<commit_message>
fix importación de excel , view
</commit_message>
<xml_diff>
--- a/public/plantillas/excel/export-catalogo-cuentas.xlsx
+++ b/public/plantillas/excel/export-catalogo-cuentas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOX0041\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\sistema-contable\public\plantillas\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FE498BE-87B5-400F-87C6-4BE5F6FC0CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0FA9E9-D038-4528-848C-6E47B9E5FBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A2AE2034-F604-4493-B048-E4A39ECD138D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>codigo</t>
   </si>
@@ -43,14 +43,25 @@
   </si>
   <si>
     <t>saldo</t>
+  </si>
+  <si>
+    <t>tipo_cuenta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90C8A6F-E1C6-407F-8162-6A60B393BDBE}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -407,7 +419,7 @@
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +438,15 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>